<commit_message>
Updated output converter to fix some bugs (still not 100% confident)
</commit_message>
<xml_diff>
--- a/pangaea/pangaea-artefact/output_converter/trainticket_results/trainticket_pangaea.xlsx
+++ b/pangaea/pangaea-artefact/output_converter/trainticket_results/trainticket_pangaea.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margara/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margara/Documents/Uni/Projects/2022_Microservices/software/cromlech/pangaea/pangaea-artefact/output_converter/trainticket_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E35448-7AAF-EC4B-8404-E178B26D7E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69B8AC5-71A2-5F40-9481-AE341D55909E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="20280" windowHeight="22500" xr2:uid="{E2AEAD66-D799-3347-B06E-FF17D0A580D3}"/>
+    <workbookView xWindow="17140" yWindow="880" windowWidth="20280" windowHeight="22500" xr2:uid="{E2AEAD66-D799-3347-B06E-FF17D0A580D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -427,7 +427,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -475,11 +475,11 @@
         <v>0.54779999999999995</v>
       </c>
       <c r="F2" s="1">
-        <v>2.8500000000000001E-2</v>
+        <v>0.24909999999999999</v>
       </c>
       <c r="G2" s="1">
-        <f>(A2*E2)-((1-A2)*F2)</f>
-        <v>2.9129999999999993E-2</v>
+        <f t="shared" ref="G2:G10" si="0">(A2*E2)-((1-A2)*F2)</f>
+        <v>-0.16941000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -499,11 +499,11 @@
         <v>0.68940000000000001</v>
       </c>
       <c r="F3" s="1">
-        <v>2.8500000000000001E-2</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="G3" s="1">
-        <f>(A3*E3)-((1-A3)*F3)</f>
-        <v>0.11508</v>
+        <f t="shared" si="0"/>
+        <v>-2.3720000000000019E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -523,11 +523,11 @@
         <v>0.74109999999999998</v>
       </c>
       <c r="F4" s="1">
-        <v>2.8500000000000001E-2</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="G4" s="1">
-        <f>(A4*E4)-((1-A4)*F4)</f>
-        <v>0.20238</v>
+        <f t="shared" si="0"/>
+        <v>8.0930000000000002E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -547,11 +547,11 @@
         <v>0.76959999999999995</v>
       </c>
       <c r="F5" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="G5" s="1">
-        <f>(A5*E5)-((1-A5)*F5)</f>
-        <v>0.29224</v>
+        <f t="shared" si="0"/>
+        <v>0.18664</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -571,11 +571,11 @@
         <v>0.82730000000000004</v>
       </c>
       <c r="F6" s="1">
-        <v>7.3999999999999996E-2</v>
+        <v>0.19950000000000001</v>
       </c>
       <c r="G6" s="1">
-        <f>(A6*E6)-((1-A6)*F6)</f>
-        <v>0.37665000000000004</v>
+        <f t="shared" si="0"/>
+        <v>0.31390000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -595,11 +595,11 @@
         <v>0.90280000000000005</v>
       </c>
       <c r="F7" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="G7" s="1">
-        <f>(A7*E7)-((1-A7)*F7)</f>
-        <v>0.53128000000000009</v>
+        <f t="shared" si="0"/>
+        <v>0.47128000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -619,11 +619,11 @@
         <v>0.90039999999999998</v>
       </c>
       <c r="F8" s="1">
-        <v>2.9700000000000001E-2</v>
+        <v>0.20069999999999999</v>
       </c>
       <c r="G8" s="1">
-        <f>(A8*E8)-((1-A8)*F8)</f>
-        <v>0.62136999999999998</v>
+        <f t="shared" si="0"/>
+        <v>0.57006999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -643,11 +643,11 @@
         <v>0.89649999999999996</v>
       </c>
       <c r="F9" s="1">
-        <v>0</v>
+        <v>0.2392</v>
       </c>
       <c r="G9" s="1">
-        <f>(A9*E9)-((1-A9)*F9)</f>
-        <v>0.71720000000000006</v>
+        <f t="shared" si="0"/>
+        <v>0.66936000000000007</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -667,11 +667,11 @@
         <v>0.90559999999999996</v>
       </c>
       <c r="F10" s="1">
-        <v>7.3999999999999996E-2</v>
+        <v>0.16109999999999999</v>
       </c>
       <c r="G10" s="1">
-        <f>(A10*E10)-((1-A10)*F10)</f>
-        <v>0.80764000000000002</v>
+        <f t="shared" si="0"/>
+        <v>0.79893000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added Pangea's trainticket architectures files to compute similarity. Added similarity in excel results.
</commit_message>
<xml_diff>
--- a/pangaea/pangaea-artefact/output_converter/trainticket_results/trainticket_pangaea.xlsx
+++ b/pangaea/pangaea-artefact/output_converter/trainticket_results/trainticket_pangaea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margara/Documents/Uni/Projects/2022_Microservices/software/cromlech/pangaea/pangaea-artefact/output_converter/trainticket_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF7EDA9-DC84-6B41-9961-6608E29B72D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58CE389-B2A2-9145-989D-11C17F333D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35920" yWindow="500" windowWidth="15280" windowHeight="27540" xr2:uid="{E2AEAD66-D799-3347-B06E-FF17D0A580D3}"/>
+    <workbookView xWindow="30600" yWindow="500" windowWidth="20600" windowHeight="27540" xr2:uid="{E2AEAD66-D799-3347-B06E-FF17D0A580D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>comm weight</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>alpha</t>
+  </si>
+  <si>
+    <t>op sim</t>
+  </si>
+  <si>
+    <t>data sim</t>
   </si>
 </sst>
 </file>
@@ -102,7 +108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -110,10 +116,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FEE5C3-71B5-2347-8C3F-BC0E15C347CA}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,7 +441,7 @@
     <col min="2" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -461,32 +463,44 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>100</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
         <v>5</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1">
         <v>0.2671</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">(A2*E2)-((1-A2)*F2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="1">
+        <v>-2.6499999999999999E-2</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.1784</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0.1</v>
       </c>
@@ -509,8 +523,14 @@
         <f t="shared" si="0"/>
         <v>-0.14592000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="1">
+        <v>0.69130000000000003</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.68700000000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0.2</v>
       </c>
@@ -533,8 +553,14 @@
         <f t="shared" si="0"/>
         <v>5.3639999999999993E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="1">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.76019999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0.3</v>
       </c>
@@ -557,8 +583,14 @@
         <f t="shared" si="0"/>
         <v>0.13035000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="1">
+        <v>0.85050000000000003</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.79669999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0.4</v>
       </c>
@@ -581,8 +613,14 @@
         <f t="shared" si="0"/>
         <v>0.22533999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="1">
+        <v>0.84530000000000005</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.81089999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0.5</v>
       </c>
@@ -605,8 +643,14 @@
         <f t="shared" si="0"/>
         <v>0.3145</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="1">
+        <v>0.87329999999999997</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.83919999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>0.6</v>
       </c>
@@ -629,8 +673,14 @@
         <f t="shared" si="0"/>
         <v>0.40636000000000005</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="1">
+        <v>0.94910000000000005</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.89239999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>0.7</v>
       </c>
@@ -653,8 +703,14 @@
         <f t="shared" si="0"/>
         <v>0.52617999999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="1">
+        <v>0.93289999999999995</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.89239999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0.8</v>
       </c>
@@ -677,8 +733,14 @@
         <f t="shared" si="0"/>
         <v>0.64806000000000008</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="1">
+        <v>0.92530000000000001</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.89239999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>0.9</v>
       </c>
@@ -701,8 +763,14 @@
         <f t="shared" si="0"/>
         <v>0.77229000000000003</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="1">
+        <v>0.94359999999999999</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.90269999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -719,7 +787,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>

</xml_diff>